<commit_message>
I updated the code to match the fleet register
</commit_message>
<xml_diff>
--- a/Data/Processed/List of illegal landings with no auction_cleaned.xlsx
+++ b/Data/Processed/List of illegal landings with no auction_cleaned.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/augustinlafond/Desktop/Dutch COVID temporary cessation payments/Data/Processed.nosync/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/augustinlafond/Desktop/projets R/duch-temporary-cessations/Data/Processed/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83091740-0712-E640-857F-1174DD60D1FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DE839B9-70FB-7744-8ADE-B7BB0A2948E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuille 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1573" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1629" uniqueCount="101">
   <si>
     <t>date</t>
   </si>
@@ -321,12 +321,15 @@
   <si>
     <t>UK242</t>
   </si>
+  <si>
+    <t>SL45</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -351,6 +354,12 @@
       <name val="Helvetica Neue"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -372,7 +381,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -425,13 +434,41 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="9"/>
+      </left>
+      <right style="thin">
+        <color indexed="9"/>
+      </right>
+      <top style="thin">
+        <color indexed="9"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -485,6 +522,26 @@
     </xf>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1643,11 +1700,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F786"/>
+  <dimension ref="A1:F814"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A745" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A711" sqref="A711:C713"/>
+      <pane ySplit="1" topLeftCell="A784" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C814" sqref="C814"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -12634,7 +12691,7 @@
       <c r="E784" s="12"/>
       <c r="F784" s="12"/>
     </row>
-    <row r="785" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="785" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A785" s="9">
         <v>44151</v>
       </c>
@@ -12649,18 +12706,410 @@
       <c r="F785" s="12"/>
     </row>
     <row r="786" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A786" s="9">
+      <c r="A786" s="19">
         <v>44165</v>
       </c>
-      <c r="B786" s="10" t="s">
+      <c r="B786" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="C786" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D786" s="12"/>
-      <c r="E786" s="12"/>
-      <c r="F786" s="12"/>
+      <c r="C786" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="D786" s="22"/>
+      <c r="E786" s="22"/>
+      <c r="F786" s="22"/>
+    </row>
+    <row r="787" spans="1:6" s="18" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A787" s="24">
+        <v>44001</v>
+      </c>
+      <c r="B787" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="C787" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="D787" s="23"/>
+      <c r="E787" s="23"/>
+      <c r="F787" s="23"/>
+    </row>
+    <row r="788" spans="1:6" s="18" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A788" s="24">
+        <v>44005</v>
+      </c>
+      <c r="B788" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="C788" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="D788" s="23"/>
+      <c r="E788" s="23"/>
+      <c r="F788" s="23"/>
+    </row>
+    <row r="789" spans="1:6" s="18" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A789" s="24">
+        <v>44008</v>
+      </c>
+      <c r="B789" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="C789" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="D789" s="23"/>
+      <c r="E789" s="23"/>
+      <c r="F789" s="23"/>
+    </row>
+    <row r="790" spans="1:6" s="18" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A790" s="24">
+        <v>44012</v>
+      </c>
+      <c r="B790" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="C790" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="D790" s="23"/>
+      <c r="E790" s="23"/>
+      <c r="F790" s="23"/>
+    </row>
+    <row r="791" spans="1:6" s="18" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A791" s="24">
+        <v>44014</v>
+      </c>
+      <c r="B791" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="C791" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="D791" s="23"/>
+      <c r="E791" s="23"/>
+      <c r="F791" s="23"/>
+    </row>
+    <row r="792" spans="1:6" s="18" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A792" s="24">
+        <v>44018</v>
+      </c>
+      <c r="B792" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="C792" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="D792" s="23"/>
+      <c r="E792" s="23"/>
+      <c r="F792" s="23"/>
+    </row>
+    <row r="793" spans="1:6" s="18" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A793" s="24">
+        <v>44021</v>
+      </c>
+      <c r="B793" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="C793" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="D793" s="23"/>
+      <c r="E793" s="23"/>
+      <c r="F793" s="23"/>
+    </row>
+    <row r="794" spans="1:6" s="18" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A794" s="24">
+        <v>44022</v>
+      </c>
+      <c r="B794" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="C794" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="D794" s="23"/>
+      <c r="E794" s="23"/>
+      <c r="F794" s="23"/>
+    </row>
+    <row r="795" spans="1:6" s="18" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A795" s="24">
+        <v>44025</v>
+      </c>
+      <c r="B795" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="C795" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="D795" s="23"/>
+      <c r="E795" s="23"/>
+      <c r="F795" s="23"/>
+    </row>
+    <row r="796" spans="1:6" s="18" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A796" s="24">
+        <v>44041</v>
+      </c>
+      <c r="B796" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="C796" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="D796" s="23"/>
+      <c r="E796" s="23"/>
+      <c r="F796" s="23"/>
+    </row>
+    <row r="797" spans="1:6" s="18" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A797" s="24">
+        <v>44043</v>
+      </c>
+      <c r="B797" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="C797" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="D797" s="23"/>
+      <c r="E797" s="23"/>
+      <c r="F797" s="23"/>
+    </row>
+    <row r="798" spans="1:6" s="18" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A798" s="24">
+        <v>44046</v>
+      </c>
+      <c r="B798" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="C798" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="D798" s="23"/>
+      <c r="E798" s="23"/>
+      <c r="F798" s="23"/>
+    </row>
+    <row r="799" spans="1:6" s="18" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A799" s="24">
+        <v>44049</v>
+      </c>
+      <c r="B799" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="C799" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="D799" s="23"/>
+      <c r="E799" s="23"/>
+      <c r="F799" s="23"/>
+    </row>
+    <row r="800" spans="1:6" s="18" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A800" s="24">
+        <v>44050</v>
+      </c>
+      <c r="B800" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="C800" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="D800" s="23"/>
+      <c r="E800" s="23"/>
+      <c r="F800" s="23"/>
+    </row>
+    <row r="801" spans="1:6" s="18" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A801" s="24">
+        <v>44053</v>
+      </c>
+      <c r="B801" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="C801" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="D801" s="23"/>
+      <c r="E801" s="23"/>
+      <c r="F801" s="23"/>
+    </row>
+    <row r="802" spans="1:6" s="18" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A802" s="24">
+        <v>44056</v>
+      </c>
+      <c r="B802" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="C802" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="D802" s="23"/>
+      <c r="E802" s="23"/>
+      <c r="F802" s="23"/>
+    </row>
+    <row r="803" spans="1:6" s="18" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A803" s="24">
+        <v>44060</v>
+      </c>
+      <c r="B803" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="C803" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="D803" s="23"/>
+      <c r="E803" s="23"/>
+      <c r="F803" s="23"/>
+    </row>
+    <row r="804" spans="1:6" s="18" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A804" s="24">
+        <v>44063</v>
+      </c>
+      <c r="B804" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="C804" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="D804" s="23"/>
+      <c r="E804" s="23"/>
+      <c r="F804" s="23"/>
+    </row>
+    <row r="805" spans="1:6" s="18" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A805" s="24">
+        <v>44067</v>
+      </c>
+      <c r="B805" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="C805" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="D805" s="23"/>
+      <c r="E805" s="23"/>
+      <c r="F805" s="23"/>
+    </row>
+    <row r="806" spans="1:6" s="18" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A806" s="24">
+        <v>44069</v>
+      </c>
+      <c r="B806" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="C806" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="D806" s="23"/>
+      <c r="E806" s="23"/>
+      <c r="F806" s="23"/>
+    </row>
+    <row r="807" spans="1:6" s="18" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A807" s="24">
+        <v>44074</v>
+      </c>
+      <c r="B807" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="C807" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="D807" s="23"/>
+      <c r="E807" s="23"/>
+      <c r="F807" s="23"/>
+    </row>
+    <row r="808" spans="1:6" s="18" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A808" s="24">
+        <v>44077</v>
+      </c>
+      <c r="B808" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="C808" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="D808" s="23"/>
+      <c r="E808" s="23"/>
+      <c r="F808" s="23"/>
+    </row>
+    <row r="809" spans="1:6" s="18" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A809" s="24">
+        <v>44081</v>
+      </c>
+      <c r="B809" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="C809" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="D809" s="23"/>
+      <c r="E809" s="23"/>
+      <c r="F809" s="23"/>
+    </row>
+    <row r="810" spans="1:6" s="18" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A810" s="24">
+        <v>44084</v>
+      </c>
+      <c r="B810" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="C810" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="D810" s="23"/>
+      <c r="E810" s="23"/>
+      <c r="F810" s="23"/>
+    </row>
+    <row r="811" spans="1:6" s="18" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A811" s="24">
+        <v>44088</v>
+      </c>
+      <c r="B811" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="C811" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="D811" s="23"/>
+      <c r="E811" s="23"/>
+      <c r="F811" s="23"/>
+    </row>
+    <row r="812" spans="1:6" s="18" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A812" s="24">
+        <v>44090</v>
+      </c>
+      <c r="B812" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="C812" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="D812" s="23"/>
+      <c r="E812" s="23"/>
+      <c r="F812" s="23"/>
+    </row>
+    <row r="813" spans="1:6" s="18" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A813" s="24">
+        <v>44095</v>
+      </c>
+      <c r="B813" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="C813" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="D813" s="23"/>
+      <c r="E813" s="23"/>
+      <c r="F813" s="23"/>
+    </row>
+    <row r="814" spans="1:6" s="18" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A814" s="24">
+        <v>44096</v>
+      </c>
+      <c r="B814" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="C814" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="D814" s="23"/>
+      <c r="E814" s="23"/>
+      <c r="F814" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.27777800000000002" footer="0.27777800000000002"/>

</xml_diff>